<commit_message>
Add QCon InfoQ scraper with multi-threading support
- Implemented a new scraper for QCon InfoQ conference agenda and abstracts.
- Utilized Selenium for web scraping with multi-threading to improve efficiency.
- Added random delays to mimic human behavior during scraping.
- Introduced a thread-safe data collection mechanism.
- Included functionality to extract PDF links associated with the conference talks.
- Created a structured output in CSV format for the scraped data.
</commit_message>
<xml_diff>
--- a/202503 AICon Shanghai_20250611.xlsx
+++ b/202503 AICon Shanghai_20250611.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2570518d-cd47-448c-8b5f-8d6e7801b441</t>
+          <t>7e981703-7509-40ef-bb9d-a6e59613d2e5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -512,7 +512,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>b1d1cf64-a595-4d1b-af39-fc0d51451ce3</t>
+          <t>e8972134-d42f-477a-9a06-9f635bc9f307</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -522,48 +522,10 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>面向端侧大模型的原生 AI SoC 设计与实践</t>
+          <t>开源大模型创新背后的 RISC-V 算力架构革新</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>随着端侧人工智能模型技术的快速发展，端侧大模型应用迎来爆发，除了端侧大模型本身，端侧大模型算力芯片平台同样面临挑战。本次演讲从大模型时代下的芯片架构，工具链，生态等方向出发，基于自研创新架构，打造适合端侧大模型高效部署推理和适合端侧产品高性价比应用的端侧芯片，赋能端侧大模型场景高性价比，高能效比的落地应用。
-演讲提纲：
-大模型技术发展给芯片带来的挑战
-传统端侧SOC VS 大模型端侧SOC
-原生大模型端侧AI SOC设计思路
-基于大模型的创新NPU架构设计
-端侧大模型+端侧SOC结合
-生态合作伙伴建设
-听众收益：
-了解大模型时代端侧芯片架构设计思路
-了解端侧芯片生态建设</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6477</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>d7d3cff1-a9fb-483a-a2e3-4c0c3ac127b3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>开源大模型创新背后的 RISC-V 算力架构革新</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>以DeepSeek为代表的开源大模型创新让普惠“满血大模型”走入千行百业成为可能，而在作为大模型应用基础的算力层面，特别是端侧推理场景，同样也已掀起了一场以开源架构实现普惠高性能算力的“革命”。
 传统算力架构因迭代缓慢、成本高昂等原因已逐渐无法适应大模型创新飞速变化的算力需求，开源、开放的RISC-V架构正成为算力架构创新的主力。本次演讲将从算力厂商的角度，介绍开源大模型创新为端侧推理算力带来的机遇与挑战，并分享RISC-V架构如何凭借开源、开放的优势，成为算力架构创新的“最终答案”。
@@ -591,21 +553,66 @@
 共同探讨开源硬件架构如何与开源大模型创新融合，造就更强大的“普惠大模型”</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6460</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5004</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20883ce7-97f2-4f68-816b-58a4b5ca089d</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>多模态大模型时空感知理解能力前沿进展</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>近年来，多模态大模型技术发展迅速，展现出强大的视觉理解能力。其中基于大模型的长视频理解任务受到了越来越多的关注，其在教育、影视、安防等领域具有广泛的应用前景。然后由于大语言模型的有效上下文长度有限，难以用有限的 GPU 计算资源实现长视频理解。
+针对这一研究问题，课题组首先推出了面向长视频理解大模型的测评基准：MLVU，提供了丰富的评测任务，揭示了主流大模型在长视频理解任务上的能力缺陷。针对长视频数据 Token 数量过多的问题，课题组提出利用可学习 Token 来自适应地压缩视频 Token，从而实现单张卡处理 1 小时以上视频的能力。
+演讲提纲：
+基于大模型的长视频理解任务与挑战
+主流的视频理解模型与能力测评
+基于可学习 Token 的视频 Token 压缩技术
+可学习的压缩 Token 
+自适应切片算法
+训练数据扩增方法
+应用实例分析
+总结与展望
+听众收益：
+了解最新的长视频理解大模型性能和局限性
+了解最新的长视频理解大模型 Token 压缩技术</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6460</t>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6388</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5004</t>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4976</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5b07e792-85ba-4c4a-b63c-ce000a502f71</t>
+          <t>bb41e42f-6916-4f9d-8256-21542fb09f07</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -646,7 +653,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>9f297ea6-a376-43ac-ab99-f2349c1f1ed9</t>
+          <t>3e528a01-04ad-43d0-b033-2964d8d43c98</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -656,55 +663,10 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>多模态大模型时空感知理解能力前沿进展</t>
+          <t>千卡级分布式集群上的视觉多模态大模型落地实践</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>近年来，多模态大模型技术发展迅速，展现出强大的视觉理解能力。其中基于大模型的长视频理解任务受到了越来越多的关注，其在教育、影视、安防等领域具有广泛的应用前景。然后由于大语言模型的有效上下文长度有限，难以用有限的 GPU 计算资源实现长视频理解。
-针对这一研究问题，课题组首先推出了面向长视频理解大模型的测评基准：MLVU，提供了丰富的评测任务，揭示了主流大模型在长视频理解任务上的能力缺陷。针对长视频数据 Token 数量过多的问题，课题组提出利用可学习 Token 来自适应地压缩视频 Token，从而实现单张卡处理 1 小时以上视频的能力。
-演讲提纲：
-基于大模型的长视频理解任务与挑战
-主流的视频理解模型与能力测评
-基于可学习 Token 的视频 Token 压缩技术
-可学习的压缩 Token 
-自适应切片算法
-训练数据扩增方法
-应用实例分析
-总结与展望
-听众收益：
-了解最新的长视频理解大模型性能和局限性
-了解最新的长视频理解大模型 Token 压缩技术</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6388</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4976</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>63218362-2702-48f0-ad40-f1cb86acb7f5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>千卡级分布式集群上的视觉多模态大模型落地实践</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>多模态大模型在智能客服、自动驾驶、AIGC 等领域的应用需求不断增长，但其训练工程面临计算、存储、数据处理、分布式通信等多重挑战。特别是在千卡级GPU 训练集群上，如何优化数据加载、提升训练稳定性、突破计算与存储瓶颈，成为AI Infra需要重点攻克的难题。本次演讲将基于LLaVA视觉多模态理解模型和FLUX文生图模型的训练工程实践，详细解析大规模GPU训练集群下的数据存储优化、分布式计算策略、训练容错机制，并探讨如何提升大规模多模态模型的训练效率和稳定性。演讲将重点介绍混合并行训练、数据高效加载、自动容错恢复等技术方案，为业界提供可落地的工程实践经验。
 演讲提纲：
@@ -725,34 +687,34 @@
 借鉴 LLaVA 和 FLUX 训练的实际优化经验，为自身多模态模型训练提供参考</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6410</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4977</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>a2546015-358c-45fc-aa67-3011867fa8f9</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>多模态理解在 AIGC 场景中的主要应用</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2ecba134-b3be-43bc-8f04-7fa7bcc23ea6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>面向端侧大模型的原生 AI SoC 设计与实践</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2024是AIGC爆发的一年。自年初OpenAI的Sora概念推出以来，各家互联网公司争相进入文生视频的赛道，AI创作出的视频愈加真实且具有美感，满足了更多影视创作和专业用户的需求。同时，生成式的搜索和推荐也逐渐进入各家电商和短视频平台的事业，将用户画像建模和意图理解准确性提升到新的高度。多模态理解技术在这些AI原生应用背后承担着支撑性的作用，显著提升了AIGC的可控性。
 本次分享将从国内外多模态理解技术的发展脉络出发，首先介绍行业的几个重点流派。随后将结合快手中的实际需求场景，讲述在技术落地过程中对疑难关键问题的思考和处理方案。同时，多模态大模型训练过程中的规模效应、模型选择、数据构造、训练范式等方面的探索也会被介绍。最后，结合短视频社交平台业务属性和创作者生态的主要关注目标，本次分享中将讨论未来多模态理解数据的发展方向和更多的应用前景。
@@ -769,6 +731,50 @@
 了解前沿多模态理解技术与业务结合的方案和思考</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6477</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4978</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dfb3e3f3-f7b4-4852-a1a6-75a54d5a52c0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>多模态理解在 AIGC 场景中的主要应用</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024是AIGC爆发的一年。自年初OpenAI的Sora概念推出以来，各家互联网公司争相进入文生视频的赛道，AI创作出的视频愈加真实且具有美感，满足了更多影视创作和专业用户的需求。同时，生成式的搜索和推荐也逐渐进入各家电商和短视频平台的事业，将用户画像建模和意图理解准确性提升到新的高度。多模态理解技术在这些AI原生应用背后承担着支撑性的作用，显著提升了AIGC的可控性。
+本次分享将从国内外多模态理解技术的发展脉络出发，首先介绍行业的几个重点流派。随后将结合快手中的实际需求场景，讲述在技术落地过程中对疑难关键问题的思考和处理方案。同时，多模态大模型训练过程中的规模效应、模型选择、数据构造、训练范式等方面的探索也会被介绍。最后，结合短视频社交平台业务属性和创作者生态的主要关注目标，本次分享中将讨论未来多模态理解数据的发展方向和更多的应用前景。
+演讲提纲：
+多模态理解技术的发展历史
+多模态理解技术中的几项代表性工作
+业务及技术挑战（效果方面及性能方面）
+工业界自研多模态模型和开源多模态模型的对比思考
+如何训练多模态大模型
+总结展望
+听众收益：
+了解多模态理解技术及案例
+了解快手AIGC背后多模态理解技术的实践经验
+了解前沿多模态理解技术与业务结合的方案和思考</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6351</t>
@@ -783,7 +789,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>9e4c9489-2963-4196-a697-e5e8911692a8</t>
+          <t>96909a18-5021-4b5d-b342-cb9f58c44394</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -830,7 +836,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>f75a42ef-d52a-4351-ba0e-c0ff11cbe088</t>
+          <t>2a3e25d9-ddaf-47c4-9395-5a57ca8959b4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -845,7 +851,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>爬取失敗，已達最大重試次數</t>
+          <t>随着大语言模型和智能体（Agent）技术的快速发展，AI Coding Agent 已成为软件开发领域的革命性力量，已从简单的代码生成工具向具备自主规划、决策和协作能力的编程助手演进。本次演讲将深入探讨AI Coding Agent的核心技术架构、落地挑战与解决方案，并分享实际场景中的实践案例。我们将从上下文体系、工具体系、评测体系、扩展性等方面阐述在 IDE 中落地 AI Agent 所需的核心能力，通过系统性技术解析与实战经验，为开发者与企业提供可复用的AI Coding Agent建设方法。
+演讲提纲：
+AI Coding 的技术演进趋势
+打造 AI Coding Agent 的核心原则
+简单 Simple
+智能 Intelligent
+主动学习 Active Learning
+核心架构设计与关键技术突破  
+企业级落地实践
+未来趋势展望
+听众收益
+掌握构建企业级 AI Coding Agent 的核心技术架构与工程实践
+获取前沿 AI 编程技术的发展趋势，为团队技术选型与规划提供参考</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -853,12 +871,16 @@
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6395</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5000</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>9c4ab856-680d-4bae-99af-7deeb6a16332</t>
+          <t>793489f3-2bd5-431a-9d33-a3728a114bf7</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -914,7 +936,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>b8c114d1-d6b1-414d-b830-5122dc2c3e42</t>
+          <t>e0fa5d4d-7546-4848-849b-90665bbad97a</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -971,7 +993,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0e797b85-0cec-4070-99f1-5c10d16bf82b</t>
+          <t>8538fc11-6fcc-4cb1-ba3c-f5e0873b0eb0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -981,58 +1003,10 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>智能体在知识库与客服的深度应用实践</t>
+          <t>Data is Power，AI is Motor</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
-        <is>
-          <t>本次演讲将深入探讨智能体技术的发展背景、核心能力及未来前景。首先我会分享智能体的定义、定位及其能力分级，重点剖析规划、记忆与自适应等关键技术，以及“Computer use”在智能体中的应用；随后，结合澜舟实践，分享大模型在企业应用中所面临的挑战，并介绍基于澜舟智搭平台的智能体解决思路和具体实施步骤。通过智能知识库和智能客服等实际案例，与你一起交流智能体在企业数智化转型中的应用价值与发展潜力。
-演讲提纲：
-智能体技术发展背景与现状
-智能体定义和定位
-智能体核心能力和水准分级
-智能体关键技术
-规划、记忆与自适应
-Computer use
-智能体技术与企业应用
-大模型在企业应用中面临的挑战
-大模型发展与局限
-大模型应用开发成本
-智能体解决方案和实施步骤
- 智能体平台与应用快速开发
-智能体具体实施步骤
-智能体应用案例分析
-智能知识库应用案例分析
-智能客服应用案例分析
-总结与展望
-听众收益：
-了解智能体相关发展背景、发展趋势和关键技术，以及智能体技术在企业数智化过程中的实际应用</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6457</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>8f9af105-50f6-41a6-8805-bea1d500b7f2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Data is Power，AI is Motor</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
         <is>
           <t>当代人工智能的发展路线的本质是数据智能。真实应用中的人工智能犹如电机（Motor），由数据这种新的能源动力（Power）驱动，助力各领域数字化变革，激发新的数字经济形态的诞生。传统的数据管理系统正从封闭的信息系统的后台走向人工智能应用的开放环境。
 演讲将讨论人工智能应用场景对于数据管理的新要求，并从系统接口、系统架构、实现技术等方面介绍技术的发展变化和新趋势。
@@ -1054,34 +1028,34 @@
 从人工智能应用角度审视数据管理系统技术体系的变化</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6427</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4986</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>40c4a5f0-bfb9-4da4-a6d0-809482a8f6a2</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3a6e6668-eeac-4bd6-86c6-0a266c65d754</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>构建下一代数据架构，释放 AI 的“数据智慧”</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>有研究表明，数据科学的工作中，仅有 20% 的精力花在了实际分析上，剩下的 80% 都投入到了数据准备上了。此外，数据准备阶段的数据质量，直接决定了模型训练的效果。因此，在 AI 时代，Data for AI 变得尤其重要，让好数据更易获取，成为企业追求的重要目标。 云原生技术与大数据技术进一步深度融合，促进了湖仓一体技术的兴起。同时 Data Fabric 等新兴数据架构的出现，给企业数据架构演进带来了新的方向。在 AI 时代，企业的的数据架构应该如何设计与演进？本次演讲将会探寻 AI 时代的现代数据架构。
 演讲提纲：
@@ -1107,172 +1081,34 @@
 了解 Lakehouse、Data Fabric 等技术在企业落地的最佳实践</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6390</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5002</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>76379903-8667-4082-aca0-dfb90fcfd37c</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Data Warebase: Instant Ingest-Transform-Explore-Retrieve for AI applications</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>我们预见未来的应用将围绕两大关键API构建：以LLM大模型为核心的智能API，以及以多模数据库为基石的数据API。Data Warebase（Data Warehouse + Database）正是这一理念的革新产品。作为新一代多模数据库引擎，它凭借三大核心技术优势：多样化的索引能力，领先的行列混存架构(实现事务处理和实时分析的高效统一，满足不同场景的查询需求)，极致的存算分离设计(提供极致的弹性扩展能力), 通过单一引擎实现数据库、数据仓库、流处理、文档存储和检索、向量检索、以及全文搜索的能力。开发者仅需使用标准SQL即可快速构建各类应用，并且永远不必担心业务规模增长带来的扩展性挑战。
-演讲提纲：
-生成式 AI 时代的数据挑战与机遇
-挑战：生成式 AI 与大模型带来的变革，数据处理需求升级
-机遇：传统数据架构的局限，多模数据库是AI时代的必然趋势
-分布式 Data Warebase 架构解析
-设计理念：用一个引擎支持大部分数据服务的需求，完美覆盖HTAP，流批一体，湖仓一体等中间态产品
-核心组件：融合数据库与数据仓库在存储和索引上的所有优点满足不同场景的查询需求，使用最先进的存算分离架构确保秒级弹性伸缩
-Data Warebase is all you need for AI application
-背景：一个完整的AI workflow包括：Ingest，Transform，Explorer，Retrieve，Act，Test，Evolve
-诠释：详尽剖析Data Warebase是如何满足所有AI workflow的需求
-实时特征工程与在线特征库
-核心需求：实时特征的高吞吐写入和查询，在线特征库在 AI 中的应用
-干货分享：实时特征工程的挑战和方案
-应用场景与案例分享
-金融（行情分析、交易、风控），车联网，互联网搜广推系统，AI Agents的数据存储，Feature Store，DevOps之数据可观测性
-听众收益：
-深入了解生成式AI时代对数据系统的核心挑战与未来机遇
-学习如何通过 Data Warebase 构建高效、实时的数据处理、存储、和多模查询的应用架构，赋能下一代 AI 应用</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6481</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>f1f0adab-0226-4b6e-8414-e02f654ce158</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Chat2Graph：Graph + AI 时代的未来智能体架构</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>随着大语言模型的兴起，如何有效地将图计算技术与人工智能技术相结合（Graph + AI），是非常值得探索的方向。一方面可以借助大模型、 智能体技术降低图计算产品的使用门槛（AI for Graph）。 另一方面，发挥图计算在关联分析场景的性能与可解释性优势，可以帮助大模型、智能体提升推理能力和生成质量（Graph for AI）。作为首个开源的Graph智能体系统，Chat2Graph充分结合了图计算与大模型技术的优势，实现了图数据库上的智能体推理增强，提升用图体验、加速方案生成、实现与图对话。
-演讲提纲
-Graph + AI 技术背景
-Graph增强的智能体架构
-Chat2Graph：首个Graph智能体
-未来展望
-听众收益
-蚂蚁图团队的 Graph + AI 开源技术实践
-如何借助图计算技术实现智能体系统能力增强
-未来智能体的架构形态与演进方向</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6507</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>7184a269-2790-4942-8ab1-6163eff6d254</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>大模型+数据资产变现，RAG 驱动企业智能化实践案例</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>在大模型进入产业深水区的今天，企业如何将大模型的强大能力真正落地于业务系统？RAG（Retrieval-Augmented Generation，检索增强生成）作为连接“数据—知识—大模型”的关键桥梁，成为构建企业智能应用的核心技术路径。
-这次演讲聚焦于企业级RAG系统的全链路技术与实践，从数据准备、文档解析、向量构建，到生成优化与评估体系，结合实际案例，系统性剖析RAG如何赋能金融、医疗、合规等多个关键领域，推动知识资产变现、提升智能问答与决策质量，助力企业迈向“知识驱动的智能体”。
-演讲提纲：
-为什么RAG是“模型×知识×数据”融合的关键？
-从大模型闭卷到开卷的转变
-为什么企业智能不能仅靠大模型本身？
-RAG作为连接业务知识与语言模型的技术桥梁
-RAG全链路技术解析：从数据到答案
-数据准备的重要性（80%的精力在数据，20%在模型）
-文档导入、结构解析、语义分块的实践挑战
-向量化、检索与生成的协同优化路径
-RAG真实应用案例拆解
-案例1：医疗术语标准化系统的落地实践
-案例2：如何实现企业文档合规性问答系统
-案例3：GraphRAG与知识图谱问答系统落地
-RAG的前沿与未来
-从RAG到Agentic RAG：检索的主动性与智能性演化
-多模态RAG、轻量图RAG等新范式探索
-企业如何构建自己的“智能体中枢”
-听众收益：
-从全局理解RAG在企业中的定位与价值
-掌握RAG系统构建的关键技术路径和优化思路
-获取真实落地经验与工具建议
-把握RAG未来发展趋势，洞察智能企业的下一站</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6473</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5003</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>42d4dba0-c74f-45a4-a60d-a9c88dc18fd7</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>07fb8f5d-91e3-4095-9465-d19e21d2c5ba</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>从技术到应用，火山引擎 Data Agent 分析智能体提效落地实践</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>从 2022 年 GPT-3.5 横空出世以来，大语言模型和 BI 系统结合以实现自然语言查数，是各家 BI 产品积极探索的方向。从 2023 年立项以来，经过多种形态的产品探索，最终在抖音集团内部取得取得初步的 PMF，并在外部得到多行业、多场景应用。本次演讲主要分享Data Agent 分析智能体的产品探索与演进、落地难点与解决方案、典型实践以及对未来产品形态的演进思考。
 演讲提纲：
@@ -1300,30 +1136,174 @@
 了解 ChatBI 智能体在数据分析中的应用，把握技术发展方向</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6352</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ee8cd42c-e971-4962-beb0-e0f069fa5df3</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>bd410b35-ffbd-415f-9ccc-9078a9f2e0d5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>智能体在知识库与客服的深度应用实践</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>本次演讲将深入探讨智能体技术的发展背景、核心能力及未来前景。首先我会分享智能体的定义、定位及其能力分级，重点剖析规划、记忆与自适应等关键技术，以及“Computer use”在智能体中的应用；随后，结合澜舟实践，分享大模型在企业应用中所面临的挑战，并介绍基于澜舟智搭平台的智能体解决思路和具体实施步骤。通过智能知识库和智能客服等实际案例，与你一起交流智能体在企业数智化转型中的应用价值与发展潜力。
+演讲提纲：
+智能体技术发展背景与现状
+智能体定义和定位
+智能体核心能力和水准分级
+智能体关键技术
+规划、记忆与自适应
+Computer use
+智能体技术与企业应用
+大模型在企业应用中面临的挑战
+大模型发展与局限
+大模型应用开发成本
+智能体解决方案和实施步骤
+ 智能体平台与应用快速开发
+智能体具体实施步骤
+智能体应用案例分析
+智能知识库应用案例分析
+智能客服应用案例分析
+总结与展望
+听众收益：
+了解智能体相关发展背景、发展趋势和关键技术，以及智能体技术在企业数智化过程中的实际应用</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6457</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5003</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>be676ccf-20b0-4039-9889-546c43879c1d</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Chat2Graph：Graph + AI 时代的未来智能体架构</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>随着大语言模型的兴起，如何有效地将图计算技术与人工智能技术相结合（Graph + AI），是非常值得探索的方向。一方面可以借助大模型、 智能体技术降低图计算产品的使用门槛（AI for Graph）。 另一方面，发挥图计算在关联分析场景的性能与可解释性优势，可以帮助大模型、智能体提升推理能力和生成质量（Graph for AI）。作为首个开源的Graph智能体系统，Chat2Graph充分结合了图计算与大模型技术的优势，实现了图数据库上的智能体推理增强，提升用图体验、加速方案生成、实现与图对话。
+演讲提纲
+Graph + AI 技术背景
+Graph增强的智能体架构
+Chat2Graph：首个Graph智能体
+未来展望
+听众收益
+蚂蚁图团队的 Graph + AI 开源技术实践
+如何借助图计算技术实现智能体系统能力增强
+未来智能体的架构形态与演进方向</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6507</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>eff91496-bdcb-453f-9736-d51cc9845b50</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>大模型+数据资产变现，RAG 驱动企业智能化实践案例</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>在大模型进入产业深水区的今天，企业如何将大模型的强大能力真正落地于业务系统？RAG（Retrieval-Augmented Generation，检索增强生成）作为连接“数据—知识—大模型”的关键桥梁，成为构建企业智能应用的核心技术路径。
+这次演讲聚焦于企业级RAG系统的全链路技术与实践，从数据准备、文档解析、向量构建，到生成优化与评估体系，结合实际案例，系统性剖析RAG如何赋能金融、医疗、合规等多个关键领域，推动知识资产变现、提升智能问答与决策质量，助力企业迈向“知识驱动的智能体”。
+演讲提纲：
+为什么RAG是“模型×知识×数据”融合的关键？
+从大模型闭卷到开卷的转变
+为什么企业智能不能仅靠大模型本身？
+RAG作为连接业务知识与语言模型的技术桥梁
+RAG全链路技术解析：从数据到答案
+数据准备的重要性（80%的精力在数据，20%在模型）
+文档导入、结构解析、语义分块的实践挑战
+向量化、检索与生成的协同优化路径
+RAG真实应用案例拆解
+案例1：医疗术语标准化系统的落地实践
+案例2：如何实现企业文档合规性问答系统
+案例3：GraphRAG与知识图谱问答系统落地
+RAG的前沿与未来
+从RAG到Agentic RAG：检索的主动性与智能性演化
+多模态RAG、轻量图RAG等新范式探索
+企业如何构建自己的“智能体中枢”
+听众收益：
+从全局理解RAG在企业中的定位与价值
+掌握RAG系统构建的关键技术路径和优化思路
+获取真实落地经验与工具建议
+把握RAG未来发展趋势，洞察智能企业的下一站</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6473</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5003</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>7d404c72-007b-48ca-8c2a-eb7bc2032420</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>金融领域大模型数据集管理与应用</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>在金融科技快速发展的当下，数据质量已成为大模型应用效果的关键因素之一。本次演讲将聚焦于灵雨平台在金融垂直领域的数据管理实践，介绍其在多源异构数据整合、高质量Chain-of-Thought（CoT）数据构建流程、多模态数据处理与质量控制等方面的技术实现。我们将详细解析平台的整体架构设计、核心算法机制与系统落地方案，分享如何构建从原始数据采集、加工到模型驱动决策的闭环体系，以支撑金融业务的智能化升级。
 演讲摘要：
@@ -1350,96 +1330,34 @@
 掌握高质量CoT数据构建与多模态数据管理方法，助力在金融场景中落地智能化应用</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6472</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4972</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>8eb34123-e4ef-4ccc-b096-cd66a0603984</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>AI 时代实验平台演进之路，从 A/B 测试到智能决策闭环</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>字节跳动A/B测试平台（内部名称Libra，对外产品DataTester）是全球领先的A/B测试与智能优化平台，累计支持超340W次实验，同时运行7W+实验，覆盖抖音、今日头条等数百业务。平台脱胎于字节跳动2012年引入的A/B测试体系，2016年实现产品化，2021年通过火山引擎开放给企业客户，融合了科学分流、智能分析、多场景特型实验等能力，成为驱动业务增长的核心基础设施。在AI时代，平台正从“功能策略验证工具”向“企业创新加速引擎”升级，探索推理模型+数据+工程的自动化决策范式。
-演讲提纲：
-传统 A/B 测试的挑战与 AI 的颠覆性机会
-传统 A/B测试的“天花板”
-人工设计依赖经验，实验效率低（如多变量组合爆炸问题）
-样本偏差与统计显著性陷阱（尤其在小流量场景）
-长反馈周期无法匹配业务实时决策需求
-AI 的颠覆性价值
-从“假设驱动”到“智能驱动”：AI 自动生成实验假设和设计、自主分析结果
-从“串行分工”到“智能协同”：面向PM、DA、RD等实验Role的AI Team协同
-从“结果验证”到“决策生成”：模拟海量用户在线实验效果提前敏捷决策
-字节跳动 A/B 测试平台的进化路径
-第一阶段：规模化实验基础设施
-超大规模和复杂场景实验引擎
-科学高效的实验科学分析引擎
-第二阶段：AI 增强的智能实验
-超参数优化：基于历史数据的贝叶斯优化，自动优化参数组合
-流量智能调优：基于多臂老虎机，在实验运行中动态调整流量
-因果推断增强：通过异质人群挖掘，自动下钻出实验影响维度
-第三阶段：决策智能体生态
-智能实验设计：通过自然语言交互定义实验假设和设计
-智能实验分析：分析智能体助力日常实验分析与写报告
-海量用户模拟：基于 AI的预实验模拟，规避策略冲突与业务风险
-未来展望：A/B 测试的终极形态
-个性化实验设计：未来的 A/B 测试将从"一刀切"的分组进化为针对不同用户精准设计的个性化实验，大幅提高实验效率和精度
-因果推断的突破：AI 系统将帮助企业从相关性分析迈向更深层次的因果推断，从"发现现象"升级为"理解原因"，为决策提供更深刻的洞察
-闭环决策系统：A/B 测试将从独立工具演变为完整的决策闭环系统，整合假设生成、实验设计、结果分析和自动执行，实现决策过程的高度自动化，进化为企业创新操作系统
-听众收益：
-战略视角：理解 AI 如何将 A/B测试从“辅助工具”升级为“决策核心”，重塑企业竞争力
-技术前瞻：掌握A/B 测试与生成式 AI、因果推断等新技术融合最新技术路径
-实践洞察：借鉴字节跳动亿级用户场景的实战经验，规避规模化实验的典型陷阱</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6476</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5006</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>3224c789-c505-48a3-99fa-673fab690d33</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>d3523528-6850-4f9c-84a0-3d8f927c3266</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>基于统一标准的智能数据治理Dataphin的落地实践</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>AI 时代数据治理面临的挑战和机会是什么？一方面 AI 的成功依赖于高质量的好数据，好数据依赖依赖于可持续的数据治理，通过基于数据标准为中心的方法论极大降低了传统数据治理方法的复杂度，从过去运动式的治理变成可持续的数据治理；另一方面数据治理的过程依赖大量的人工，AI 赋能数据治理，帮助把重度依赖人工的数据治理变得自动化和智能化。面对 AI 时代，通过 AI 赋能，叠加可持续的数据治理方法论，让好数据加持业务创新和发展。
 演讲提纲：
@@ -1476,17 +1394,141 @@
 了解AI如何为数据治理提效</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6363</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>b9ea8274-d34c-4ce1-8d7e-c7b7a780fa4d</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Data Warebase: Instant Ingest-Transform-Explore-Retrieve for AI applications</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>字节跳动A/B测试平台（内部名称Libra，对外产品DataTester）是全球领先的A/B测试与智能优化平台，累计支持超340W次实验，同时运行7W+实验，覆盖抖音、今日头条等数百业务。平台脱胎于字节跳动2012年引入的A/B测试体系，2016年实现产品化，2021年通过火山引擎开放给企业客户，融合了科学分流、智能分析、多场景特型实验等能力，成为驱动业务增长的核心基础设施。在AI时代，平台正从“功能策略验证工具”向“企业创新加速引擎”升级，探索推理模型+数据+工程的自动化决策范式。
+演讲提纲：
+传统 A/B 测试的挑战与 AI 的颠覆性机会
+传统 A/B测试的“天花板”
+人工设计依赖经验，实验效率低（如多变量组合爆炸问题）
+样本偏差与统计显著性陷阱（尤其在小流量场景）
+长反馈周期无法匹配业务实时决策需求
+AI 的颠覆性价值
+从“假设驱动”到“智能驱动”：AI 自动生成实验假设和设计、自主分析结果
+从“串行分工”到“智能协同”：面向PM、DA、RD等实验Role的AI Team协同
+从“结果验证”到“决策生成”：模拟海量用户在线实验效果提前敏捷决策
+字节跳动 A/B 测试平台的进化路径
+第一阶段：规模化实验基础设施
+超大规模和复杂场景实验引擎
+科学高效的实验科学分析引擎
+第二阶段：AI 增强的智能实验
+超参数优化：基于历史数据的贝叶斯优化，自动优化参数组合
+流量智能调优：基于多臂老虎机，在实验运行中动态调整流量
+因果推断增强：通过异质人群挖掘，自动下钻出实验影响维度
+第三阶段：决策智能体生态
+智能实验设计：通过自然语言交互定义实验假设和设计
+智能实验分析：分析智能体助力日常实验分析与写报告
+海量用户模拟：基于 AI的预实验模拟，规避策略冲突与业务风险
+未来展望：A/B 测试的终极形态
+个性化实验设计：未来的 A/B 测试将从"一刀切"的分组进化为针对不同用户精准设计的个性化实验，大幅提高实验效率和精度
+因果推断的突破：AI 系统将帮助企业从相关性分析迈向更深层次的因果推断，从"发现现象"升级为"理解原因"，为决策提供更深刻的洞察
+闭环决策系统：A/B 测试将从独立工具演变为完整的决策闭环系统，整合假设生成、实验设计、结果分析和自动执行，实现决策过程的高度自动化，进化为企业创新操作系统
+听众收益：
+战略视角：理解 AI 如何将 A/B测试从“辅助工具”升级为“决策核心”，重塑企业竞争力
+技术前瞻：掌握A/B 测试与生成式 AI、因果推断等新技术融合最新技术路径
+实践洞察：借鉴字节跳动亿级用户场景的实战经验，规避规模化实验的典型陷阱</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6481</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5006</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>bfa1956f-67f7-4b8d-8880-1a28428b34d0</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AI 时代实验平台演进之路，从 A/B 测试到智能决策闭环</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>字节跳动A/B测试平台（内部名称Libra，对外产品DataTester）是全球领先的A/B测试与智能优化平台，累计支持超340W次实验，同时运行7W+实验，覆盖抖音、今日头条等数百业务。平台脱胎于字节跳动2012年引入的A/B测试体系，2016年实现产品化，2021年通过火山引擎开放给企业客户，融合了科学分流、智能分析、多场景特型实验等能力，成为驱动业务增长的核心基础设施。在AI时代，平台正从“功能策略验证工具”向“企业创新加速引擎”升级，探索推理模型+数据+工程的自动化决策范式。
+演讲提纲：
+传统 A/B 测试的挑战与 AI 的颠覆性机会
+传统 A/B测试的“天花板”
+人工设计依赖经验，实验效率低（如多变量组合爆炸问题）
+样本偏差与统计显著性陷阱（尤其在小流量场景）
+长反馈周期无法匹配业务实时决策需求
+AI 的颠覆性价值
+从“假设驱动”到“智能驱动”：AI 自动生成实验假设和设计、自主分析结果
+从“串行分工”到“智能协同”：面向PM、DA、RD等实验Role的AI Team协同
+从“结果验证”到“决策生成”：模拟海量用户在线实验效果提前敏捷决策
+字节跳动 A/B 测试平台的进化路径
+第一阶段：规模化实验基础设施
+超大规模和复杂场景实验引擎
+科学高效的实验科学分析引擎
+第二阶段：AI 增强的智能实验
+超参数优化：基于历史数据的贝叶斯优化，自动优化参数组合
+流量智能调优：基于多臂老虎机，在实验运行中动态调整流量
+因果推断增强：通过异质人群挖掘，自动下钻出实验影响维度
+第三阶段：决策智能体生态
+智能实验设计：通过自然语言交互定义实验假设和设计
+智能实验分析：分析智能体助力日常实验分析与写报告
+海量用户模拟：基于 AI的预实验模拟，规避策略冲突与业务风险
+未来展望：A/B 测试的终极形态
+个性化实验设计：未来的 A/B 测试将从"一刀切"的分组进化为针对不同用户精准设计的个性化实验，大幅提高实验效率和精度
+因果推断的突破：AI 系统将帮助企业从相关性分析迈向更深层次的因果推断，从"发现现象"升级为"理解原因"，为决策提供更深刻的洞察
+闭环决策系统：A/B 测试将从独立工具演变为完整的决策闭环系统，整合假设生成、实验设计、结果分析和自动执行，实现决策过程的高度自动化，进化为企业创新操作系统
+听众收益：
+战略视角：理解 AI 如何将 A/B测试从“辅助工具”升级为“决策核心”，重塑企业竞争力
+技术前瞻：掌握A/B 测试与生成式 AI、因果推断等新技术融合最新技术路径
+实践洞察：借鉴字节跳动亿级用户场景的实战经验，规避规模化实验的典型陷阱</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6363</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6476</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5006</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>45b8e858-482d-4bd6-b16a-16e68379619f</t>
+          <t>6f1ee707-4a95-403a-99fb-3bc2143ed443</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1496,17 +1538,18 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>开场致辞</t>
+          <t>推理 Scaling Law 在音乐大模型 Mureka 中的应用与创新</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>爬取失敗，已達最大重試次數</t>
+          <t>本次将分享Chain-of-Thought（CoT）技术和推理能力引入到音乐生成模型中的开发进展。
+Mureka O1 中包含了Mureka团队最新发布的音乐生成领域的创新研究成果——MusiCoT。MusiCoT利用了思维链Chain-of-Thought （CoT）方法，不同于传统自回归模型逐步生成音频，MusiCoT首次在细粒度音频token预测前预生成整体音乐结构，大幅提升生成音乐的结构连贯性与乐器编排精准度。同时基于CLAP模型，无需人工标注即具备高扩展性，并显著提高了生成音乐的可解释性和质量。MusiCoT为高保真AI音乐生成开辟全新路径，推动音乐AI创作迈入结构化时代。</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6524</t>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6491</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1514,7 +1557,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>66264a8b-cad0-495f-987a-94bbd84ed354</t>
+          <t>64cc5446-34d1-43d3-8c5a-c6304b4d1a89</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1524,26 +1567,29 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>推理 Scaling Law 在音乐大模型 Mureka 中的应用与创新</t>
+          <t>AI 重构全球数字基建：从统一底座到多云协同的技术跃迁</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>本次将分享Chain-of-Thought（CoT）技术和推理能力引入到音乐生成模型中的开发进展。
-Mureka O1 中包含了Mureka团队最新发布的音乐生成领域的创新研究成果——MusiCoT。MusiCoT利用了思维链Chain-of-Thought （CoT）方法，不同于传统自回归模型逐步生成音频，MusiCoT首次在细粒度音频token预测前预生成整体音乐结构，大幅提升生成音乐的结构连贯性与乐器编排精准度。同时基于CLAP模型，无需人工标注即具备高扩展性，并显著提高了生成音乐的可解释性和质量。MusiCoT为高保真AI音乐生成开辟全新路径，推动音乐AI创作迈入结构化时代。</t>
+          <t>演讲将系统展示美的在AI大模型、基础设施平台、大数据平台、数据库管理、研发效能优化、自动化运维等领域的创新实践，涵盖从技术架构设计到实际业务落地的全链条解决方案。通过美的的数字化转型三阶段（业务数字化，数字化驱动业务，全球化+AI深化）及海外拓展案例，揭示如何通过统一底座实现“多云”环境下的高效协同与安全管控，并重点分享AI大模型在数据分析、智能协作、自动化运维等场景中的深度融合应用。本次分享不仅是一次头部企业技术全景的深度拆解，更将为AI开发者、企业决策者及技术管理者提供从架构设计到组织协同的完整数字化转型框架，推动全球AI产业在技术突破与商业落地之间的高效衔接。</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6491</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6506</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4970</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>32555aa6-4700-4a73-af3f-2e2f52008db5</t>
+          <t>47377a17-fe96-4620-b710-2602451e199b</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1571,7 +1617,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4521057e-7a6b-4371-bb26-f14628baba6b</t>
+          <t>6c30eb2d-c4ef-45c1-9e51-a5fc7fb17e70</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1599,7 +1645,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>bf8f80e0-45c1-4e81-ab01-5865add49c7e</t>
+          <t>c59e9815-24e6-45a0-bf3d-5dc4d5438eb3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1609,42 +1655,10 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AI 重构全球数字基建：从统一底座到多云协同的技术跃迁</t>
+          <t>开场致辞</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
-        <is>
-          <t>演讲将系统展示美的在AI大模型、基础设施平台、大数据平台、数据库管理、研发效能优化、自动化运维等领域的创新实践，涵盖从技术架构设计到实际业务落地的全链条解决方案。通过美的的数字化转型三阶段（业务数字化，数字化驱动业务，全球化+AI深化）及海外拓展案例，揭示如何通过统一底座实现“多云”环境下的高效协同与安全管控，并重点分享AI大模型在数据分析、智能协作、自动化运维等场景中的深度融合应用。本次分享不仅是一次头部企业技术全景的深度拆解，更将为AI开发者、企业决策者及技术管理者提供从架构设计到组织协同的完整数字化转型框架，推动全球AI产业在技术突破与商业落地之间的高效衔接。</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6506</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4970</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>62d6dbad-120f-489d-96df-cb78c4470494</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>解耦与互联：ADK、MCP、A2A 如何重塑 Agent 开发与协作范式</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
         <is>
           <t>实现能够解决复杂业务问题的并具备企业级稳健性的 Agent 架构，面临开发复杂、工具集成缺失、协同难的难点。本次分享将重点介绍 Agent Development Kit (ADK)、Model Context Protocol (MCP) 和 Agent2Agent Protocol (A2A) 三大创新技术如何重塑 Agent 的开发与协作范式。您将看到 ADK 如何简化 Agent 的开发与编排 ，MCP 如何标准化 Agent 与工具及数据的交互 ，以及 A2A 如何实现 Agent 间的协作 。我们还将通过一个实战演示展示这三者如何协同作用，构建出模块化、可扩展、企业级的下一代 Agent 架构，为开发者和架构师提供构建下一代智能解决方案的清晰蓝图和实践指导。
 演讲提纲：
@@ -1667,6 +1681,52 @@
 熟悉使用 ADK+MCP+A2A 构建多 Agent 的实战经验</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6524</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>becf4f3a-05c0-4803-b9a3-d44196023bf8</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>解耦与互联：ADK、MCP、A2A 如何重塑 Agent 开发与协作范式</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>实现能够解决复杂业务问题的并具备企业级稳健性的 Agent 架构，面临开发复杂、工具集成缺失、协同难的难点。本次分享将重点介绍 Agent Development Kit (ADK)、Model Context Protocol (MCP) 和 Agent2Agent Protocol (A2A) 三大创新技术如何重塑 Agent 的开发与协作范式。您将看到 ADK 如何简化 Agent 的开发与编排 ，MCP 如何标准化 Agent 与工具及数据的交互 ，以及 A2A 如何实现 Agent 间的协作 。我们还将通过一个实战演示展示这三者如何协同作用，构建出模块化、可扩展、企业级的下一代 Agent 架构，为开发者和架构师提供构建下一代智能解决方案的清晰蓝图和实践指导。
+演讲提纲：
+1. 企业级 AI Agent 的发展机遇与架构挑战
+2. ADK 重塑 Agent 开发和部署
+ADK 设计理念：模块化、可控性与开发者体验 
+ADK 的核心支柱：构建、交互、评估、部署
+3. MCP 赋能 Agent 与世界的连接
+MCP 主要用来解决什么问题
+MCP 架构和工作原理
+4. A2A 实现 Agent 之间通信和协作
+A2A 通过新的协议和自然语言简化 Agent 到 Agent 的协作
+A2A 如何进行 能力发现，任务管理，数据交互，相互协商
+5. ADK + MCP + A2A 构建企业级 Agent 实践
+演示多个 Agent 如何进行协作
+6. Agent 未来展望
+听众受益：
+理解企业级Agent在实际落地中的挑战与解决思路
+掌握 ADK, MCP, A2A 三大前沿技术
+熟悉使用 ADK+MCP+A2A 构建多 Agent 的实战经验</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6520</t>
@@ -1677,7 +1737,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>85026b99-7462-4a50-a98d-a2f647fe7c53</t>
+          <t>a69465f8-0157-41f6-8da6-0df54901bdc7</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1760,7 +1820,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>a81fa8de-c97b-44e6-87e1-100f6da02eba</t>
+          <t>d327dd3c-0bcc-426a-9e81-a39175e9f14d</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1803,7 +1863,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>881c81cc-5ccc-4331-a7d2-1932fd4e7258</t>
+          <t>f99d77b0-c07e-4b07-8d23-f3f0b524744f</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1813,65 +1873,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>华为昇腾推理技术的优化实践</t>
+          <t>腾讯混元 AngelHCF 推理加速框架优化实践</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
-        <is>
-          <t>随着大模型技术的快速发展，其在LLM、多模态融合等领域的应用越来越广泛。然而，大模型的高效推理仍然是一个关键挑战，从计算复杂度、内存占用、通信技术等各个技术层面展开，如何在保证性能的同时降低计算成本、提升推理效率成为了关键挑战。
-本次演讲将围绕大模型推理优化的技术发展方向，围绕模型层、推理框架层、算子层这3个方面展开，并结合实践案例，阐述相关的技术方案和选型，帮助听众更好地理解和应用大模型推理技术。
-演讲提纲：
-大模型推理加速的技术挑战与常用方案
-算子融合，如 FA，通算融合
-模型量化，如 w8a8 等
-Attention容量压缩，如 MLA、GQA 等
-技术研究热点：模型层、框架层、算子层
-模型层优化
-昇腾推理领域加速库ATB
-推理框架层优化
-- 昇腾图编译技术TorchAir
-- PD分离部署
-- 动态批处理（Dynamic Batching）、Prefix Cache等
-算子层优化
-高效融合算子，如MLA算子设计
-NPU 亲和性编程，充分利用 Cube 和 Vector 计算单元能力
-业务实践：推理优化成功案例
-通信融合算子最大化时间掩盖，如 AllGatherMatmul
-MLAPO大融合算子，加速降低计算耗时
-下一步优化方向
-PD+大EP 等
-听众收益：
-了解当前华为昇腾推理技术的优化实践</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6433</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4999</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>083945ef-a50f-4f6a-810a-0d798dfe01b3</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>腾讯混元 AngelHCF 推理加速框架优化实践</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
         <is>
           <t>腾讯 AngelHCF 推理加速框架针对混元 LLM 大语言模型做了深度推理优化，结合全新的 Hybrid 模型结构整体上取得了不错的推理成本优势，支撑了元宝线上混元模型上万卡推理。同时，AngelHCF于24 年初即大规模部署上线了万亿 MoE 大模型，针对大规模MoE模型通信特点做了混合切分策略优化，叠加模型压缩、PD 分离等优化手段，显著降低了线上推理成本。本次分享将从不同角度分别介绍腾讯混元推理加速框架 AngelHCF 所做的一些针对性优化，结合全新的Turbos 模型结构，希望能给听众带来一些新的启发。
 演讲提纲：
@@ -1894,30 +1899,30 @@
 了解大规模 MoE 语言模型推理加速具体方法&amp;实践</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6440</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>aecc2539-3298-4557-b6b2-2b175e2775f3</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>5362f780-e146-492e-8fa0-6d9f80eef11a</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
         <is>
           <t>超越算力瓶颈，大模型推理的跨层优化前沿实践</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>本次演讲将带领大家逐层解析大模型推理的核心技术。从模型代码讲解 Transformer 前向传播的核心流程与关键模块设计；框架层解读主流推理引擎（如 vLLM/TensorRT）的加速原理与适用场景；深度学习框架揭示 PyTorch 动态图编译、算子优化等底层支持技术；硬件加速剖析 CUDA 并行计算与内存优化策略；最后结合 GPU 特性分析不同硬件对推理性能的影响规律，提供从代码优化到硬件选型的全链路实践指南，帮助开发者快速构建高效推理方案。
 演讲提纲：
@@ -1946,9 +1951,60 @@
 了解最前沿的推理优化技术和技术局限性</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6418</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>08801d59-828e-4194-b868-d02c2de56b87</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>华为昇腾推理技术的优化实践</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>随着大模型技术的快速发展，其在LLM、多模态融合等领域的应用越来越广泛。然而，大模型的高效推理仍然是一个关键挑战，从计算复杂度、内存占用、通信技术等各个技术层面展开，如何在保证性能的同时降低计算成本、提升推理效率成为了关键挑战。
+本次演讲将围绕大模型推理优化的技术发展方向，围绕模型层、推理框架层、算子层这3个方面展开，并结合实践案例，阐述相关的技术方案和选型，帮助听众更好地理解和应用大模型推理技术。
+演讲提纲：
+大模型推理加速的技术挑战与常用方案
+算子融合，如 FA，通算融合
+模型量化，如 w8a8 等
+Attention容量压缩，如 MLA、GQA 等
+技术研究热点：模型层、框架层、算子层
+模型层优化
+昇腾推理领域加速库ATB
+推理框架层优化
+- 昇腾图编译技术TorchAir
+- PD分离部署
+- 动态批处理（Dynamic Batching）、Prefix Cache等
+算子层优化
+高效融合算子，如MLA算子设计
+NPU 亲和性编程，充分利用 Cube 和 Vector 计算单元能力
+业务实践：推理优化成功案例
+通信融合算子最大化时间掩盖，如 AllGatherMatmul
+MLAPO大融合算子，加速降低计算耗时
+下一步优化方向
+PD+大EP 等
+听众收益：
+了解当前华为昇腾推理技术的优化实践</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6418</t>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6433</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1956,7 +2012,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>b8d8a3ce-5fc1-481c-b25a-6fa96d20a876</t>
+          <t>c2daea67-ec4e-4ec8-9cd4-c91f1d7c628b</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2008,7 +2064,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>e2452916-e35a-403a-ae64-fdf15c075aa1</t>
+          <t>6210af34-bf45-45a1-94e5-55cb16c2d533</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2069,7 +2125,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05d85a48-5d15-4d94-8984-bd74ef8e5e27</t>
+          <t>2eec0da6-7ded-47b9-b6d1-2234d161a93d</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2079,10 +2135,67 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>AI + 风控，大模型驱动金融风险决策新范式</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>大模型技术兴起，以数据为燃料、AI 为引擎的决策智能，正逐渐演变成为金融科技下一阶段的发展趋势，人工智能这么火，该如何应用到金融业务风险决策中去，也是近期金融行业讨论的一个热点话题。
+同盾科技基于大模型技术的新应用，既可以实现多模态知识抽取，从多源、多模态的富文本数据中提取客户、关联、风险事件等各类知识，更加高效地消除信息差，增加内部决策的智能性和透明化；也可以基于大模型强大的知识推理能力用于信用评估、欺诈检测等内容，引入大模型的语义识别及分析能力进行趋势研判和特征寻优。提供更简洁、高效、智能的风险识别、归因分析，实现从风险浓度的动态量化到风险态势的自动收敛。
+本次分享将围绕“AI+ 风控“，讲解大模型如何在金融风控中实践与探索，希望对你有所启发。
+演讲提纲：
+金融风控与决策智能的演变
+金融风控的趋势及变化
+决策智能，数据+AI即是新武器 
+AI重新定义风险决策智能新范式
+大模型驱动的范式革新  
+核心能力突破 
+多模态知识抽取与风险因子挖掘  
+决策推理驱动的风险动态量化与主动收敛  
+起于AI，用于智能：学会与AI协作的风控实践  
+基于富文本数据的风险态势感知
+监管科技相关的知识库建设
+专家知识与AI决策的融合方法论
+特征寻优、策略推荐及模型迭代逻辑  
+挑战与突破：如何构建可信AI风控体系
+数据隐私、模型可解释性、决策时效等核心问题  
+如何设计 MaaS 新模式
+可信 AI 的智策解决思路
+总结与未来展望
+听众收益：
+了解关于“AI+风控“的新思路和新尝试
+了解金融风控大模型的实践内容与应用成果
+了解大模型在金融风险决策中的商业化思考</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6449</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4975</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>5721e100-0902-4eaf-8ebc-5295b795726d</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>AI 给人寿保险业带来了什么？进化还是颠覆？</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>通过 AI 发展历史过程中一些关键问题的突破，探索 AI 在金融保险行业里的创新应用及商业价值；在金融保险全价值链上，LLM 模型及多模态的方案选型、技术挑战突破，及应用价值。
 演讲提纲：
@@ -2110,74 +2223,17 @@
 了解DeepSeek如何赋能寿险业务流程，在销售、培训、理赔等场景中提效提质，助力数字化转型</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6448</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>4e629534-7953-47cb-b53f-02b47fa3a512</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>AI + 风控，大模型驱动金融风险决策新范式</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>大模型技术兴起，以数据为燃料、AI 为引擎的决策智能，正逐渐演变成为金融科技下一阶段的发展趋势，人工智能这么火，该如何应用到金融业务风险决策中去，也是近期金融行业讨论的一个热点话题。
-同盾科技基于大模型技术的新应用，既可以实现多模态知识抽取，从多源、多模态的富文本数据中提取客户、关联、风险事件等各类知识，更加高效地消除信息差，增加内部决策的智能性和透明化；也可以基于大模型强大的知识推理能力用于信用评估、欺诈检测等内容，引入大模型的语义识别及分析能力进行趋势研判和特征寻优。提供更简洁、高效、智能的风险识别、归因分析，实现从风险浓度的动态量化到风险态势的自动收敛。
-本次分享将围绕“AI+ 风控“，讲解大模型如何在金融风控中实践与探索，希望对你有所启发。
-演讲提纲：
-金融风控与决策智能的演变
-金融风控的趋势及变化
-决策智能，数据+AI即是新武器 
-AI重新定义风险决策智能新范式
-大模型驱动的范式革新  
-核心能力突破 
-多模态知识抽取与风险因子挖掘  
-决策推理驱动的风险动态量化与主动收敛  
-起于AI，用于智能：学会与AI协作的风控实践  
-基于富文本数据的风险态势感知
-监管科技相关的知识库建设
-专家知识与AI决策的融合方法论
-特征寻优、策略推荐及模型迭代逻辑  
-挑战与突破：如何构建可信AI风控体系
-数据隐私、模型可解释性、决策时效等核心问题  
-如何设计 MaaS 新模式
-可信 AI 的智策解决思路
-总结与未来展望
-听众收益：
-了解关于“AI+风控“的新思路和新尝试
-了解金融风控大模型的实践内容与应用成果
-了解大模型在金融风险决策中的商业化思考</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6449</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4975</t>
-        </is>
-      </c>
+      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0fc708f7-a878-4e63-bcae-4b2cf859fbd0</t>
+          <t>8732630f-c53f-4f93-bb39-3618bd3183ad</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2187,56 +2243,10 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>快手代码大模型 Kwaipilot 在研发领域的落地实践</t>
+          <t>从 Copilot 到 Coding Agent，AI 驱动软件开发的未来</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
-        <is>
-          <t>快手自研代码大模型 Kwaipilot 正式发布，截止到目前，新增代码的AI生成率达20%。通过构建代码形式化表征和逻辑推理，实践 MoE 架构、“编码即标注”数据飞轮，在快手私域代码的理解和生成场景上，表现优于外部模型，自研代码续写模型 KwaiCoder-23BA4-v1 达到行业 SOTA 水平。
-本次演讲将从数据收集、模型训练、产品交互、落地实践多个维度介绍在快手研发领域落地代码生成大模型的实践经历。以及如何激发与结合大模型的推理能力，有效利用研发环节中的暗知识，完成研发场景下的端到端需求生存任务。
-演讲提纲：
-Kwaipiot在哪些研发场景下进行了AI研发提效？
-Kwaipiot在代码生成，端到端需求交付领域的应用
-Kwaipilot在智能cr，测试生成，智能 oncall 场景的应用
- Kwaipilot 如何协调模型和产品的关系，打造最佳用处体验的研发提效工具
- 如何平衡模型的推理成本与性能
- 如何结合使用场景构造大模型训练需要的语料数据
- 哪些因素在影响产品最终的用户体验？
-总结与展望
-听众收益：
-了解大模型可以在哪些研发流程赋能
-了解如何转起数据飞轮不断提升模型能力
-学习如何使模型具备自我反思与推理能力</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6370</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4983</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>3344800f-557a-4ba1-84fc-52c70612cd37</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>从 Copilot 到 Coding Agent，AI 驱动软件开发的未来</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
         <is>
           <t>随着 GitHub Copilot、Cursor 等工具的日益普及，越来越多的代码开始由 AI 产生。但现有模式始终困于「Copilot」范式——开发者仍需深度介入上下文、逻辑设计与调试纠偏。这种半自动化协创虽提升局部效率，却未能真正释放 AI 的工程潜能。
 本演讲将从 Copilot 的历史讲起，与听众探讨未来 Agent 如何演进，介绍当前 Coding Agent 赛道的主要方向。并讨论在 AI 重度参与软件工程过程中后，开发者在其中的位置，以及在 AI 加速软件开发过程的情况下，软件质量所碰到的挑战。最后，将介绍 Gru.ai 在开发 Coding Agent 方面的一些实践经验。
@@ -2260,34 +2270,34 @@
 了解 Coding Agent 的架构选择与开发中的取舍</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6391</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4984</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>589e8f98-0483-4f2a-af10-1406bb02676d</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>24d513af-029c-4aa3-81f3-6cbe5e75f610</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
         <is>
           <t>60K Stars 的开源 AI 产品是如何炼成的 —— 两人两年的 AI 驱动研发之旅</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>本演讲将分享利用 AI 技术打造开源 AI Chat 应用 LobeChat 并获得 59K Star 的实践经验。我们将深入剖析如何将 AI 融入产品设计 &amp; 研发全流程：例如从 AI 生成单元测试提升代码质量、实现自动国际化；从 AI 辅助技术架构决策提高选型效率，到 AI 参与项目架构设计，解决技术难题。通过真实的应用 AI 研发的演进案例，展示大模型如何赋能产研团队，实现高效率、高质量的产品研发，为开源社区贡献优质解决方案。
 演讲提纲：
@@ -2311,21 +2321,63 @@
 获取开源项目从 0 开始增长的实战经验，学习如何利用 AI 打造高质量产品</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6498</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4985</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>9c865c04-dfa7-4426-9573-85d7660a9638</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>快手代码大模型 Kwaipilot 在研发领域的落地实践</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>快手自研代码大模型 Kwaipilot 正式发布，截止到目前，新增代码的AI生成率达20%。通过构建代码形式化表征和逻辑推理，实践 MoE 架构、“编码即标注”数据飞轮，在快手私域代码的理解和生成场景上，表现优于外部模型，自研代码续写模型 KwaiCoder-23BA4-v1 达到行业 SOTA 水平。
+本次演讲将从数据收集、模型训练、产品交互、落地实践多个维度介绍在快手研发领域落地代码生成大模型的实践经历。以及如何激发与结合大模型的推理能力，有效利用研发环节中的暗知识，完成研发场景下的端到端需求生存任务。
+演讲提纲：
+Kwaipiot在哪些研发场景下进行了AI研发提效？
+Kwaipiot在代码生成，端到端需求交付领域的应用
+Kwaipilot在智能cr，测试生成，智能 oncall 场景的应用
+ Kwaipilot 如何协调模型和产品的关系，打造最佳用处体验的研发提效工具
+ 如何平衡模型的推理成本与性能
+ 如何结合使用场景构造大模型训练需要的语料数据
+ 哪些因素在影响产品最终的用户体验？
+总结与展望
+听众收益：
+了解大模型可以在哪些研发流程赋能
+了解如何转起数据飞轮不断提升模型能力
+学习如何使模型具备自我反思与推理能力</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6498</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4985</t>
-        </is>
-      </c>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6370</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3c4bd124-a403-4fcc-ba6b-c13f901f93ef</t>
+          <t>a3e2973d-e3c1-40cc-a2e3-0262be64052e</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2369,7 +2421,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6374b427-ccda-441f-a4dd-ce1896aa3fbd</t>
+          <t>4cdfbee2-7699-4c83-bc54-df8e7fe24f75</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2410,7 +2462,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>933d1629-377d-417c-9c33-10d66cda641d</t>
+          <t>6cb352b0-7c0c-4ae8-97ec-a65f88528013</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2455,7 +2507,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>537f908b-994e-45a7-b138-dbf3e6ad9ed8</t>
+          <t>ee6a310d-f5f0-47b5-9bbc-12926955947a</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2465,95 +2517,10 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>阿里云客户服务领域Agent在业务提效上的思考与创新实践</t>
+          <t>AI 原生时代，搜索引擎的范式重构与产品哲学</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
-        <is>
-          <t>随着 AI Agent 技术的快速发展，业界许多企业开始在 Agent 方向进行深层次的探索，而不仅仅是停留在“大模型 + 工具调用”的简单应用上。在经过近 1 年的技术探索，我们在阿里云客户服务业务的需求和 Agent 行业快速发展的双驱动下，摸索了一套在客户服务领域高效构建 Agent 和 Multi-Agent 协同模式，可以快速赋能业务提效的方法论，并基于此自研建设了“阿里云服务领域 Agent 平台”，用于更快速、低成本的构建出适合于客服业务场景使用的各类 Agent，更快的帮助业务提效、解决痛点问题。
-本次演讲，我们将首先介绍 Agent 的技术本质、业界常见的类型、模式，Agent 技术对客服领域的价值增益，然后分析阿里云服务领域业务中的痛点，再来介绍我们是如何使用 Agent 技术来赋能阿里云的客户服务业务场景，展示服务领域 Agent 技术具体落地实践效果，以及我们是如何自研的领域 Agent 平台，我们希望这些思考和设计思路，能给各行业听众起到一些抛砖引玉的作用。
-演讲提纲：
-Agent技术本质与常见模式
-Agent技术对客户服务领域的价值增益
-阿里云服务领域的业务背景与要求
-阿里云服务领域Agent的设计方法论与落地效果
-阿里云服务领域Agent平台的设计与思考
-听众收益：
-了解在阿里云客户服务这个垂类领域中Agent方向的技术探索
-客户服务领域Agent高效构建过程的方法论</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6502</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4998</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>815e7965-1e3e-419e-b52a-0287c80a603d</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>生成式 AI 在产品设计和 UI 领域：过去、现在和未来</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>产品设计界面无处不在，从我们每天接触的手机、车载屏幕到各种智能设备。如今，生成式 AI 已在文字、图片、视频带来了诸多改变，它在 UI 领域又会产生哪些深远影响？作为身处在这个行业之中的创业者，我将在本次演讲向你分享我们对过去的观察、思考和未来的展望，并向你演示这个领域的生成效果、产品化等随模型进展演进的过程。
-我将结合过去，将生成式 AI 在 UI 领域的阶段分为四个象限，分别称为“玩具”初稿、模板商店、灵感涌现和新的范式阶段。在介绍这四个象限的同时，我也将向你详述过去“套模板”技术路线的利弊，基础模型在 AI Coding 能力上的溢出对这个行业的影响，并详细的向你分享这个过程中产品路径、技术的变化，我们收获的经验和反思。
-演讲提纲：
-初代生成式 UI：“玩具” 初稿，“套模板” 技术路线
-基础模型 AI Coding 能力溢出：表达力从简单到复杂，灵感涌现
-基于设计系统的 UI 生成
-四种假设：未来的界面设计编辑器将如何演进
-设计与研发的角色变化：未来的我们是谁
-听众收益：
-新的经验：AI 时代做产品，Bet 什么
-理解产品定义-设计-研发新流程，为自己团队工作流提效提供有效思路
-研习当下最热门的 AI 产研类工具，理解本质，更好应用于自己工作</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6482</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4982</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>ebfb20a4-fbc9-45ad-a722-44c225e238ab</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>AI 原生时代，搜索引擎的范式重构与产品哲学</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
         <is>
           <t>随着AGI（通用人工智能）的发展，传统搜索引擎的局限性日益凸显：基于关键字的检索模式难以理解用户深层意图，且缺乏语义关联性，导致信息整合效率低下。同时，AGI对高质量数据的需求激增，但互联网公共数据逐渐枯竭，低质量内容泛滥，传统SEO（搜索引擎优化）策略已无法适应AI搜索的新范式。博查AI搜索提出“新一代AI搜索引擎”架构，以混合检索（向量+关键词）和语义重排为核心，结合EEAT原则（专业性、经验、权威性、可信度）优化内容权重。同时，引入生成引擎优化（GEO）框架，通过提升内容权威性、添加统计数据及引用来源，增强生成式AI对优质内容的引用概率。本次演讲姜分享搜索引擎的范式重构与产品哲学。
 演讲提纲：
@@ -2572,9 +2539,90 @@
 发现人机协作新职业机会与商业创新的潜在领域</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6505</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ab69ae14-b737-49d8-bf00-aff8d475b6cb</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>生成式 AI 在产品设计和 UI 领域：过去、现在和未来</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>产品设计界面无处不在，从我们每天接触的手机、车载屏幕到各种智能设备。如今，生成式 AI 已在文字、图片、视频带来了诸多改变，它在 UI 领域又会产生哪些深远影响？作为身处在这个行业之中的创业者，我将在本次演讲向你分享我们对过去的观察、思考和未来的展望，并向你演示这个领域的生成效果、产品化等随模型进展演进的过程。
+我将结合过去，将生成式 AI 在 UI 领域的阶段分为四个象限，分别称为“玩具”初稿、模板商店、灵感涌现和新的范式阶段。在介绍这四个象限的同时，我也将向你详述过去“套模板”技术路线的利弊，基础模型在 AI Coding 能力上的溢出对这个行业的影响，并详细的向你分享这个过程中产品路径、技术的变化，我们收获的经验和反思。
+演讲提纲：
+初代生成式 UI：“玩具” 初稿，“套模板” 技术路线
+基础模型 AI Coding 能力溢出：表达力从简单到复杂，灵感涌现
+基于设计系统的 UI 生成
+四种假设：未来的界面设计编辑器将如何演进
+设计与研发的角色变化：未来的我们是谁
+听众收益：
+新的经验：AI 时代做产品，Bet 什么
+理解产品定义-设计-研发新流程，为自己团队工作流提效提供有效思路
+研习当下最热门的 AI 产研类工具，理解本质，更好应用于自己工作</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6482</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4982</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>6ec79d1a-ac62-40ea-b87f-44afa0527dac</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>阿里云客户服务领域Agent在业务提效上的思考与创新实践</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>随着 AI Agent 技术的快速发展，业界许多企业开始在 Agent 方向进行深层次的探索，而不仅仅是停留在“大模型 + 工具调用”的简单应用上。在经过近 1 年的技术探索，我们在阿里云客户服务业务的需求和 Agent 行业快速发展的双驱动下，摸索了一套在客户服务领域高效构建 Agent 和 Multi-Agent 协同模式，可以快速赋能业务提效的方法论，并基于此自研建设了“阿里云服务领域 Agent 平台”，用于更快速、低成本的构建出适合于客服业务场景使用的各类 Agent，更快的帮助业务提效、解决痛点问题。
+本次演讲，我们将首先介绍 Agent 的技术本质、业界常见的类型、模式，Agent 技术对客服领域的价值增益，然后分析阿里云服务领域业务中的痛点，再来介绍我们是如何使用 Agent 技术来赋能阿里云的客户服务业务场景，展示服务领域 Agent 技术具体落地实践效果，以及我们是如何自研的领域 Agent 平台，我们希望这些思考和设计思路，能给各行业听众起到一些抛砖引玉的作用。
+演讲提纲：
+Agent技术本质与常见模式
+Agent技术对客户服务领域的价值增益
+阿里云服务领域的业务背景与要求
+阿里云服务领域Agent的设计方法论与落地效果
+阿里云服务领域Agent平台的设计与思考
+听众收益：
+了解在阿里云客户服务这个垂类领域中Agent方向的技术探索
+客户服务领域Agent高效构建过程的方法论</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6505</t>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6502</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -2582,7 +2630,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2aaafa02-ee44-4e23-86d8-46fbc4ce1a46</t>
+          <t>249b6e26-e0e0-45f5-acc0-d3da896cdbcf</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2592,10 +2640,94 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>复杂场景下的语音交互，多模态降噪技术的实践与应用</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>在智能硬件快速发展的今天，嘈杂环境下的语音采集问题已成为制约用户体验的关键瓶颈。传统降噪技术主要依赖单模态信号处理（如麦克风阵列或数字信号处理算法），但在面对突发性噪音、多声源混叠以及动态场景时，其性能往往难以满足需求。为解决这一难题，本次演讲将重点介绍基于多模态融合的降噪技术体系。该技术通过整合麦克风阵列、摄像头视觉分析以及其他传感器数据，结合深度学习模型，实现了对复杂场景下目标声源的精准提取和背景噪音的有效抑制。
+目前，这项技术已成功应用于多种智能硬件产品中，包括大屏一体机、人形机器人、智能音箱等。通过硬件与软件的深度协同，多模态降噪技术不仅显著提升了设备在嘈杂环境中的语音识别能力，还为智能硬件的交互体验带来了质的飞跃。本次演讲将从技术原理、应用场景及未来发展方向等方面，全面解析多模态降噪技术如何应用于下一代智能硬件中。
+演讲提纲：
+多模态简介
+多模态降噪技术介绍
+单模态降噪介绍
+单模态降噪的优缺点
+多模态降噪介绍
+多模态降噪技术应用实践
+未来的工作
+听众收益
+了解如何解决嘈杂环境的收音问题
+了解麦克风阵列降噪的优缺点
+了解多模态降噪的原理和应用</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6452</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2343ca81-108d-43e7-9025-1f3816918ae1</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>大模型催化下的 AI 学习硬件演化</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>开年以来，DeepSeek-R1 推理模型将 AI 浪潮推向新的高度，各行各业迅速跟进落地。其中，网易有道作为国内领先的教育科技企业，率先推出深度融合 DeepSeek-R1 推理能力的全新品类——全面屏答疑笔【有道 SpaceOne】。作为国内首款 AI 原生学习硬件，有道 SpaceOne 将 AI 能力与教育场景、知识库优势结合，解锁学科难题深度讲解新方式，以大模型时代智能硬件的全新形态，为用户带来了超越真人老师的答疑辅导体验。
+那么，SpaceOne 如何解决答疑辅导这个难度非常大的场景问题呢？在模型能力上，子曰加 DeepSeek 的搭配会有什么不一样的效果？又为什么要以“答疑笔”这样的硬件形态出现呢？这款新形态硬件背后的考量，既浓缩了有道开创智能词典笔品类以来多年的积累与沉淀，也反映了加速迭代的 AI 技术对硬件设计与创新的挑战，蕴含了新的机遇，也提出了新的命题。
+本次演讲，将系统性地介绍便携式 AI 学习硬件【词典笔】的底层技术特点、场景应用、技术沿革，以及到新形态【答疑笔】所包含的承上启下的技术思考、突破与发展方向探索。
+演讲提纲：
+产品设计与硬件落地
+选择从“词典笔”到“答疑笔”硬件形态创新的用户洞察
+AI原生学习硬件中，从技术到产品的一体化设计
+AI Agent与教育生态的深度融合
+AI Agent重构教育场景中人、工具、内容和流程的关系
+软硬件、知识库和教育场景的深度融合
+AI学习硬件的关键突破与思考
+大模型带来的AI新方向在教育硬件中的结合和落地
+听众收益：
+作为新型AI学习硬件【词典笔】的由来与技术特点拆解
+大模型技术在便携性型硬件上落地的实践经验分享
+教育科技企业对未来AI学习硬件的认知与思考</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6479</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>06b91450-a124-48c5-b170-d7f020ff0557</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>AI 重塑游戏世界的四阶段革命，从《麦琪的花园》看未来游戏发展新范式</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>本次演讲将以《麦琪的花园》为实例，深入探讨 AI 技术如何从根本上改变游戏开发与玩家体验。首先解析游戏行业 AI 应用的四阶段发展路径（AINovel、AINPC、AIUGC、AIGC），并定位当前行业所处阶段。随后分享《麦琪的花园》开发过程中如何突破 AI 生成 NPC 的技术壁垒，实现玩家通过照片创建个性化 NPC，并赋予其自主社交、行为决策能力的实践经验。
 深入剖析"全要素生成"概念如何影响未来游戏设计，使游戏从内容导向型转变为提供底座型，内容由玩家社区与游戏自行生长，最终实现真正意义上的"无限游戏"。同时，分享小型团队如何在 AI 游戏赛道与大厂竞争并保持创新活力的经验，为中小团队提供宝贵的发展思路。
@@ -2627,103 +2759,17 @@
 获取中小团队 AI 落地路径与创新策略</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6441</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4980</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>7d9d0388-00f9-4094-b815-befb1ecd1094</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>复杂场景下的语音交互，多模态降噪技术的实践与应用</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>在智能硬件快速发展的今天，嘈杂环境下的语音采集问题已成为制约用户体验的关键瓶颈。传统降噪技术主要依赖单模态信号处理（如麦克风阵列或数字信号处理算法），但在面对突发性噪音、多声源混叠以及动态场景时，其性能往往难以满足需求。为解决这一难题，本次演讲将重点介绍基于多模态融合的降噪技术体系。该技术通过整合麦克风阵列、摄像头视觉分析以及其他传感器数据，结合深度学习模型，实现了对复杂场景下目标声源的精准提取和背景噪音的有效抑制。
-目前，这项技术已成功应用于多种智能硬件产品中，包括大屏一体机、人形机器人、智能音箱等。通过硬件与软件的深度协同，多模态降噪技术不仅显著提升了设备在嘈杂环境中的语音识别能力，还为智能硬件的交互体验带来了质的飞跃。本次演讲将从技术原理、应用场景及未来发展方向等方面，全面解析多模态降噪技术如何应用于下一代智能硬件中。
-演讲提纲：
-多模态简介
-多模态降噪技术介绍
-单模态降噪介绍
-单模态降噪的优缺点
-多模态降噪介绍
-多模态降噪技术应用实践
-未来的工作
-听众收益
-了解如何解决嘈杂环境的收音问题
-了解麦克风阵列降噪的优缺点
-了解多模态降噪的原理和应用</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6452</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>29196d93-7872-4496-bd2b-97f66433780a</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>WAKE-AI 大模型如何赋能 AI 智能眼镜的多场景应用</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>AI智能眼镜浪潮下，李未可科技基于自研的WAKE-AI多模态大模型平台，融合多模态交互、端云结合架构和轻量化硬件设计，打造了一款重新定义智能硬件的AI眼镜。本演讲将深入探讨李未可AI眼镜的核心WAKE-AI大模型平台，是如何赋能AI智能眼镜实现多场景下的落地应用。通过这些技术突破，李未可打造的AI智能眼镜智能化水平得到了有效的提升，从而实现为用户提供了全天候、高精度的智能交互体验。
-演讲提纲：
-为什么眼镜会成为AI硬件落地的最佳载体
-李未可科技AI眼镜的核心技术与产品特点
-自研WAKE-AI大模型如何赋能AI智能眼镜的多场景应用
-WAKE-AI大模型平台的多智能体系统架构
-未来展望：AI 智能眼镜将如何改变生活
-听众收益：
-了解 AI 智能眼镜的技术突破与场景潜力
-把握未来人机交互趋势与行业变革方向</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6456</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5007</t>
-        </is>
-      </c>
+      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>42752214-c79d-45eb-b55d-d1e36ce50870</t>
+          <t>c7ab139b-10ce-4dd4-aa2e-2d81a6fb4a49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2733,53 +2779,10 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>大模型催化下的 AI 学习硬件演化</t>
+          <t>AI 驱动组织进化与人才跃迁：大模型重塑企业知识工程与培训新范式</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
-        <is>
-          <t>开年以来，DeepSeek-R1 推理模型将 AI 浪潮推向新的高度，各行各业迅速跟进落地。其中，网易有道作为国内领先的教育科技企业，率先推出深度融合 DeepSeek-R1 推理能力的全新品类——全面屏答疑笔【有道 SpaceOne】。作为国内首款 AI 原生学习硬件，有道 SpaceOne 将 AI 能力与教育场景、知识库优势结合，解锁学科难题深度讲解新方式，以大模型时代智能硬件的全新形态，为用户带来了超越真人老师的答疑辅导体验。
-那么，SpaceOne 如何解决答疑辅导这个难度非常大的场景问题呢？在模型能力上，子曰加 DeepSeek 的搭配会有什么不一样的效果？又为什么要以“答疑笔”这样的硬件形态出现呢？这款新形态硬件背后的考量，既浓缩了有道开创智能词典笔品类以来多年的积累与沉淀，也反映了加速迭代的 AI 技术对硬件设计与创新的挑战，蕴含了新的机遇，也提出了新的命题。
-本次演讲，将系统性地介绍便携式 AI 学习硬件【词典笔】的底层技术特点、场景应用、技术沿革，以及到新形态【答疑笔】所包含的承上启下的技术思考、突破与发展方向探索。
-演讲提纲：
-产品设计与硬件落地
-选择从“词典笔”到“答疑笔”硬件形态创新的用户洞察
-AI原生学习硬件中，从技术到产品的一体化设计
-AI Agent与教育生态的深度融合
-AI Agent重构教育场景中人、工具、内容和流程的关系
-软硬件、知识库和教育场景的深度融合
-AI学习硬件的关键突破与思考
-大模型带来的AI新方向在教育硬件中的结合和落地
-听众收益：
-作为新型AI学习硬件【词典笔】的由来与技术特点拆解
-大模型技术在便携性型硬件上落地的实践经验分享
-教育科技企业对未来AI学习硬件的认知与思考</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6479</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ee184d08-7381-4af8-8924-b1698ef6dccd</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>AI 驱动组织进化与人才跃迁：大模型重塑企业知识工程与培训新范式</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
         <is>
           <t>在 AI 技术重构商业规则的当下，组织效能的提升与人才能力的重塑已成为企业穿越数智化深水区的核心命题。平安知鸟基于大模型技术，构建了“知识萃取 - 智能应用 - 效能提升”的闭环生态，为企业提供从知识管理到人才培养的全链路解决方案。通过深度挖掘企业隐性知识资产、构建统一知识库，并结合 AI 导师、AI 陪练等创新工具，平安知鸟不仅解决了传统培训中知识更新滞后、技能转化低效等痛点，更以“知识即生产力”的理念推动组织与人才的协同进化。本演讲将结合金融业、零售业、汽车制造业等多领域实践案例，解析大模型如何通过知识工程重构企业竞争力，为组织效能跃迁与人才能力升级提供可复用的方法论。
 演讲提纲：
@@ -2810,30 +2813,30 @@
 认识到 AI 技能对金融人的重要性，激发自主学习与工具运用意识</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6489</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>d1974f76-6e83-4f55-85db-66eb8be4f864</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
+      <c r="F50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>9274e00a-2469-4913-9fc7-6be2e92adbc3</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
         <is>
           <t>AI 时代的人才管理双螺旋，技能升级 × 心智刷新</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>面对人工智能的冲击，企业的人才发展需构建"技能升级"与"心智刷新"缠绕的双螺旋模型。AI 替代基础工作、参与工作流，带来传统“岗位适配理论”失效，更通过"任务重构"重塑职业生态——企业需求从"寻找现成答案的人"转向"提出新问题的人"+“解决复杂问题的人”。
 1.“技能升级”强调从单一硬技能转向"π型能力跃迁"，即深耕垂直领域的同时，培养跨界整合（如商业洞察 + 伦理判断）的复合素质。
@@ -2853,30 +2856,30 @@
 了解在 VUCA、BANI 及 AI 时代，如何构建竞争力，增强职业定力，减少职场焦虑，实现稳定成长</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6434</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>d1a24b86-7ad4-41a1-9b87-6135c8aa28d1</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
+      <c r="F51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>e5e37ae3-0a90-450b-9527-2ea5bec9ecda</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
         <is>
           <t>腾讯云顾问：从人到数智平台，用 AI 重塑 SRE</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>演讲围绕腾讯云 SRE 组织变革展开。在主动服务体系遇瓶颈时，腾讯云依托 AI 和云计算推出腾讯云顾问数智平台，涵盖智能生图、架构量化评估等功能。还分享了技术、组织等多方面经验，用 AI 重塑 SRE，助力其应对复杂环境挑战。
 演讲提纲：
@@ -2901,21 +2904,65 @@
 更可借鉴多维经验，涵盖技术、组织、管理、协作、技能等方面，提升个人与团队竞争力</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6480</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4981</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>73ce1a3c-214b-488f-a4de-9468472ec71a</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>GMI Cloud 全球化高性能分布式推理服务构建实践</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>AI应用全球化浪潮下， 推理效率与算力供给成为破局关键。本次演讲以GMI Cloud Inference Engine为锚点，拆解其高并发、低延迟、动态扩缩容能力如何支撑全球AI业务爆发，深度分享GMI Cloud自研推理平台的架构设计、跨区域合规部署及软硬协同优化实践，揭秘其实现推理成本、指数级效率提升的关键路径。
+演讲提纲：
+AI应用爆发背景下模型推理服务的核心挑战分析
+GMI Cloud推理优化技术分享
+单集群内推理服务自动扩容技术
+跨集群跨地区的推理服务自动扩容技术
+单集群的PD分离技术
+基于共享持久化存储的跨集群PD分离技术
+推理参数自动化评测工具介绍
+推理服务全面主动监控技术
+推理服务的自动容错恢复
+GMI Cloud Inference Engine 落地实践
+听众收益：
+明晰AI应用爆发时，模型推理服务在效率与算力上存在核心挑战
+深度了解GMI Cloud的推理优化技术，如自动扩容、PD分离、评测监控及容错恢复等
+知悉GMI Cloud Inference Engine如何动态应对高并发，保障数据处理，精准评估与监控推理服务
+复制GMI Cloud Inference Engine的优秀实践到自身业务中</t>
+        </is>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6480</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4981</t>
-        </is>
-      </c>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6486</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>25e3e75c-d97f-4e26-bb75-ac9c89da1625</t>
+          <t>40ec8d21-0611-476e-be4c-fa3c09839f77</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2925,60 +2972,10 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>开源基础设施软件如何实现全球化：从零到一亿美元 ARR 的增长之路</t>
+          <t>中国科技企业出海，要不要把新加坡作为第一站？</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
-        <is>
-          <t>Kong 最初专注于 API Marketplace 领域，随后战略转型为一家覆盖 API 全生命周期管理的公司。凭借在微服务、云原生到 AI 浪潮中的持续演进，Kong 构建起涵盖 API 网关、服务网格、API 测试工具在内的完整生态体系，逐步发展为估值 20 亿美元的全球领先企业。  
-在这次分享中，我会讲述 Kong 在成长过程中所面临的一些关键挑战，以及我们是如何把握住技术趋势，将多个核心组件整合为一个统一、协同的战略平台。此外，我还会分享 Kong 如何从零起步，实现超过 1 亿美元的年经常性收入（ARR），并通过平台化战略将产品销售到全球市场。 面对 AI 的新一轮技术革命，Kong 又是如何快速定位自身为 AI 网关的代表性产品，并持续推动产品能力演进，确保我们在这个变革时代依然保持行业领先地位。
-演讲提纲：
-背景介绍
-战略转型与生态构建
-早期挑战：专注 API Marketplace，遇到市场变化与竞争压力
-转型升级：布局全生命周期 API 管理，推出 Kong Gateway、Kuma、Insomnia 等产品
-生态构建：打造 API 网关 + 服务网格 + 测试工具的完整生态，服务微服务与云原生架构
-增长路径解析
-Product-Market Fit：以用户反馈驱动产品优化
-销售体系建设：构建全球化销售网络，推动平台化销售战略
-全球扩张：设立海外研发与支持中心，强化本地服务能力
-AI 时代的技术布局
-AI Gateway 发布：支持主流 LLM 接入，服务企业 AI 应用需求
-合规与治理工具：提升 AI 使用的安全性、可控性与可观测性
-总结与未来展望
-API + AI 融合趋势：推动企业更深层次的数字化转型
-持续创新与引领：Kong 如何保持技术领先和市场领导力
-成功经验总结
-听众收益：
-了解开源 Infra 的商业化的实践
-全球市场包括出海的一个 GTM 营销策略
-全球 AI 发展下的商业化的实践经验</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6488</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>40f7753c-cc49-4e96-b792-58a9495ee239</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>中国科技企业出海，要不要把新加坡作为第一站？</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
         <is>
           <t>在全球化日益复杂的今天，中国科技企业如何走出国门？是先立足本土再图海外，还是直奔欧美主战场？本次演讲将由白鲸开源创始人、资深开源布道者郭炜亲自讲述他在中国深耕市场后，如何打磨产品、拓展全球市场的真实经历，并分享其在新加坡、美国实地调研中得到的出海思考。通过a路径（中国→东南亚→全球）与b路径（美国→全球）的对比分析，深入探讨软件产品本地化、PMF验证、品牌构建、市场连接等关键问题，帮助中国科技创业者找到适合自己的“活路”和“出路”。如果你正在创业，或你的公司正处于产品出海、市场选择的十字路口，本场演讲将带来方向性的启发。
 演讲提纲：
@@ -3006,78 +3003,34 @@
 通过实际案例掌握如何在中国做产品化公司，并利用开源、社区等非传统打法建立品牌和用户生态</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>https://aicon.infoq.cn/2025/shanghai/presentation/6496</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4973</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>d5fd520b-5a27-4d3d-9629-e9a3ee8a512e</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>GMI Cloud 全球化高性能分布式推理服务构建实践</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>AI应用全球化浪潮下， 推理效率与算力供给成为破局关键。本次演讲以GMI Cloud Inference Engine为锚点，拆解其高并发、低延迟、动态扩缩容能力如何支撑全球AI业务爆发，深度分享GMI Cloud自研推理平台的架构设计、跨区域合规部署及软硬协同优化实践，揭秘其实现推理成本、指数级效率提升的关键路径。
-演讲提纲：
-AI应用爆发背景下模型推理服务的核心挑战分析
-GMI Cloud推理优化技术分享
-单集群内推理服务自动扩容技术
-跨集群跨地区的推理服务自动扩容技术
-单集群的PD分离技术
-基于共享持久化存储的跨集群PD分离技术
-推理参数自动化评测工具介绍
-推理服务全面主动监控技术
-推理服务的自动容错恢复
-GMI Cloud Inference Engine 落地实践
-听众收益：
-明晰AI应用爆发时，模型推理服务在效率与算力上存在核心挑战
-深度了解GMI Cloud的推理优化技术，如自动扩容、PD分离、评测监控及容错恢复等
-知悉GMI Cloud Inference Engine如何动态应对高并发，保障数据处理，精准评估与监控推理服务
-复制GMI Cloud Inference Engine的优秀实践到自身业务中</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6486</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>173270c4-2abb-4b52-a5cb-aba2c3813077</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>202503 AICon Shanghai</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>7987779d-065e-4aa6-abb7-466e36eaa156</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
         <is>
           <t>新一代智能化 B2B 电商出海的落地探索</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>本次演讲将聚焦 B2B 出海从流量获取、多语言交互到合规交易的全链路挑战，拆解 AI 驱动的技术架构与业务实践。
 演讲提纲：
@@ -3105,14 +3058,96 @@
 学习全球地址解析、动态合规风控、OFAC名单识别及智能合同生成等技术，打造合规交易全链路闭环管理体系</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6384</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4974</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>414878c1-80d4-4f52-92db-ce54d136d4b4</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>WAKE-AI 大模型如何赋能 AI 智能眼镜的多场景应用</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>AI智能眼镜浪潮下，李未可科技基于自研的WAKE-AI多模态大模型平台，融合多模态交互、端云结合架构和轻量化硬件设计，打造了一款重新定义智能硬件的AI眼镜。本演讲将深入探讨李未可AI眼镜的核心WAKE-AI大模型平台，是如何赋能AI智能眼镜实现多场景下的落地应用。通过这些技术突破，李未可打造的AI智能眼镜智能化水平得到了有效的提升，从而实现为用户提供了全天候、高精度的智能交互体验。
+演讲提纲：
+为什么眼镜会成为AI硬件落地的最佳载体
+李未可科技AI眼镜的核心技术与产品特点
+自研WAKE-AI大模型如何赋能AI智能眼镜的多场景应用
+WAKE-AI大模型平台的多智能体系统架构
+未来展望：AI 智能眼镜将如何改变生活
+听众收益：
+了解 AI 智能眼镜的技术突破与场景潜力
+把握未来人机交互趋势与行业变革方向</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6456</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5007</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>744dd54e-503c-4ba9-bcb2-ed78b2933027</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>202503 AICon Shanghai</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>开源基础设施软件如何实现全球化：从零到一亿美元 ARR 的增长之路</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>AI智能眼镜浪潮下，李未可科技基于自研的WAKE-AI多模态大模型平台，融合多模态交互、端云结合架构和轻量化硬件设计，打造了一款重新定义智能硬件的AI眼镜。本演讲将深入探讨李未可AI眼镜的核心WAKE-AI大模型平台，是如何赋能AI智能眼镜实现多场景下的落地应用。通过这些技术突破，李未可打造的AI智能眼镜智能化水平得到了有效的提升，从而实现为用户提供了全天候、高精度的智能交互体验。
+演讲提纲：
+为什么眼镜会成为AI硬件落地的最佳载体
+李未可科技AI眼镜的核心技术与产品特点
+自研WAKE-AI大模型如何赋能AI智能眼镜的多场景应用
+WAKE-AI大模型平台的多智能体系统架构
+未来展望：AI 智能眼镜将如何改变生活
+听众收益：
+了解 AI 智能眼镜的技术突破与场景潜力
+把握未来人机交互趋势与行业变革方向</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6384</t>
+          <t>https://aicon.infoq.cn/2025/shanghai/presentation/6488</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=4974</t>
+          <t>http://ppt.geekbang.org/slide/download?cid=158&amp;pid=5007</t>
         </is>
       </c>
     </row>

</xml_diff>